<commit_message>
Update to test datasets
</commit_message>
<xml_diff>
--- a/data/testdata/surname.xlsx
+++ b/data/testdata/surname.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/juan_russy_urosario_edu_co/Documents/initial_graph_repository/namegraph/data/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89AA035E-6AA2-4C49-BA8B-28C723C0A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{89AA035E-6AA2-4C49-BA8B-28C723C0A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{952BD6CB-C8A3-4A85-905B-10CDB85EE82B}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="3225" windowWidth="21600" windowHeight="10065" xr2:uid="{D7B29601-E893-4FC5-884B-B1C1A0256C03}"/>
+    <workbookView xWindow="2415" yWindow="4755" windowWidth="21600" windowHeight="11505" xr2:uid="{D7B29601-E893-4FC5-884B-B1C1A0256C03}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="102">
   <si>
     <t>cedula</t>
   </si>
@@ -228,9 +228,6 @@
     <t>MARIANA</t>
   </si>
   <si>
-    <t>DEL SOAL</t>
-  </si>
-  <si>
     <t>LUCERO</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>DE LA PARRA</t>
   </si>
   <si>
-    <t xml:space="preserve"> PATRICIA</t>
-  </si>
-  <si>
     <t>GOMEZ</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
     <t>TOMAS ARLES</t>
   </si>
   <si>
-    <t>DE LA ROSA</t>
-  </si>
-  <si>
     <t>LAVERDE</t>
   </si>
   <si>
@@ -291,15 +282,9 @@
     <t>SANTIAGO</t>
   </si>
   <si>
-    <t>DE LA CUEVA</t>
-  </si>
-  <si>
     <t>EDWARD</t>
   </si>
   <si>
-    <t>DE LA TORRE</t>
-  </si>
-  <si>
     <t>LUIS ARMANDO</t>
   </si>
   <si>
@@ -312,12 +297,6 @@
     <t>JOSEFA</t>
   </si>
   <si>
-    <t>DE LA PAZ</t>
-  </si>
-  <si>
-    <t>LUZ</t>
-  </si>
-  <si>
     <t>BART</t>
   </si>
   <si>
@@ -333,9 +312,6 @@
     <t>CECILIA</t>
   </si>
   <si>
-    <t>MARGARET</t>
-  </si>
-  <si>
     <t>DE ALBA</t>
   </si>
   <si>
@@ -343,6 +319,27 @@
   </si>
   <si>
     <t>TATIANA</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>DE_LA_CUEVA</t>
+  </si>
+  <si>
+    <t>DE DE LA BARRERA LUZ</t>
+  </si>
+  <si>
+    <t>DEL ROSAL</t>
+  </si>
+  <si>
+    <t>PATRICIA</t>
+  </si>
+  <si>
+    <t>DE_LA_TORRE</t>
+  </si>
+  <si>
+    <t>MARGARET EVELYN</t>
   </si>
 </sst>
 </file>
@@ -695,19 +692,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8586E9D3-8C93-4FF0-ADD5-B2B2B4BB3EB8}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:H97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -759,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -785,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -811,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -837,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -863,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -889,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -915,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -941,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -967,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -993,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1019,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1045,7 +1043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1071,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1097,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1149,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1175,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1227,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1253,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1276,10 +1274,10 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1299,13 +1297,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1313,11 +1311,11 @@
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1331,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1342,7 +1340,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1</v>
@@ -1357,19 +1355,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1383,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1391,11 +1389,11 @@
         <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1409,18 +1407,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1</v>
@@ -1435,18 +1433,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>1</v>
@@ -1461,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1472,7 +1470,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>1</v>
@@ -1487,18 +1485,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>1</v>
@@ -1507,24 +1505,24 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>1</v>
@@ -1539,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1547,11 +1545,11 @@
         <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1576,7 +1574,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>1</v>
@@ -1591,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1599,10 +1597,10 @@
         <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -1617,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1625,10 +1623,10 @@
         <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>1</v>
@@ -1637,13 +1635,13 @@
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1651,10 +1649,10 @@
         <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -1669,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1678,7 +1676,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>1</v>
@@ -1687,13 +1685,13 @@
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1711,22 +1709,22 @@
         <v>1</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1</v>
@@ -1735,13 +1733,13 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1750,7 +1748,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>1</v>
@@ -1759,13 +1757,13 @@
         <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1777,10 +1775,10 @@
         <v>57</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>1</v>
@@ -1789,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1798,7 +1796,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>1</v>
@@ -1807,13 +1805,13 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1822,7 +1820,7 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>1</v>
@@ -1831,13 +1829,13 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1846,7 +1844,7 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>1</v>
@@ -1855,13 +1853,13 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1870,7 +1868,7 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>1</v>
@@ -1879,13 +1877,13 @@
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1894,13 +1892,13 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>1</v>
@@ -1909,22 +1907,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>1</v>
@@ -1933,16 +1931,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>1</v>
@@ -1951,21 +1949,1235 @@
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dataset uptadte - non important
</commit_message>
<xml_diff>
--- a/data/testdata/surname.xlsx
+++ b/data/testdata/surname.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/juan_russy_urosario_edu_co/Documents/initial_graph_repository/namegraph/data/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{89AA035E-6AA2-4C49-BA8B-28C723C0A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{952BD6CB-C8A3-4A85-905B-10CDB85EE82B}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{89AA035E-6AA2-4C49-BA8B-28C723C0A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DBA8D86-B994-435D-AB38-27A2ED1E4CB8}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="4755" windowWidth="21600" windowHeight="11505" xr2:uid="{D7B29601-E893-4FC5-884B-B1C1A0256C03}"/>
+    <workbookView xWindow="4065" yWindow="2370" windowWidth="21600" windowHeight="8760" xr2:uid="{D7B29601-E893-4FC5-884B-B1C1A0256C03}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="104">
   <si>
     <t>cedula</t>
   </si>
@@ -96,18 +96,12 @@
     <t>DE LA OSSA</t>
   </si>
   <si>
-    <t>KAREN FERNANDA</t>
-  </si>
-  <si>
     <t>DEL ROZAL</t>
   </si>
   <si>
     <t>DE LA GUARDIA</t>
   </si>
   <si>
-    <t>CONSUELO</t>
-  </si>
-  <si>
     <t>DE LA BARRERA</t>
   </si>
   <si>
@@ -192,48 +186,12 @@
     <t>DE LA RENTA</t>
   </si>
   <si>
-    <t>SARA</t>
-  </si>
-  <si>
-    <t>MARJORIE JACQUELINE</t>
-  </si>
-  <si>
-    <t>MARGARITA</t>
-  </si>
-  <si>
-    <t>CARLOTA SOFIA</t>
-  </si>
-  <si>
-    <t>ROSALBA</t>
-  </si>
-  <si>
     <t>DORA</t>
   </si>
   <si>
-    <t>RAMONA</t>
-  </si>
-  <si>
-    <t>PAULA</t>
-  </si>
-  <si>
-    <t>LISA MARIE</t>
-  </si>
-  <si>
-    <t>CARLA</t>
-  </si>
-  <si>
     <t>DEL CORAL</t>
   </si>
   <si>
-    <t>MARIANA</t>
-  </si>
-  <si>
-    <t>LUCERO</t>
-  </si>
-  <si>
-    <t>FEDERICA</t>
-  </si>
-  <si>
     <t>YEPES</t>
   </si>
   <si>
@@ -246,9 +204,6 @@
     <t>DE LA ESPRIELLA</t>
   </si>
   <si>
-    <t>MARIA</t>
-  </si>
-  <si>
     <t>DE LA CALLE</t>
   </si>
   <si>
@@ -294,24 +249,12 @@
     <t>JUAN</t>
   </si>
   <si>
-    <t>JOSEFA</t>
-  </si>
-  <si>
     <t>BART</t>
   </si>
   <si>
     <t>MARIO</t>
   </si>
   <si>
-    <t>LEONOR</t>
-  </si>
-  <si>
-    <t>JULIA</t>
-  </si>
-  <si>
-    <t>CECILIA</t>
-  </si>
-  <si>
     <t>DE ALBA</t>
   </si>
   <si>
@@ -324,22 +267,85 @@
     <t>False</t>
   </si>
   <si>
-    <t>DE_LA_CUEVA</t>
-  </si>
-  <si>
     <t>DE DE LA BARRERA LUZ</t>
   </si>
   <si>
     <t>DEL ROSAL</t>
   </si>
   <si>
-    <t>PATRICIA</t>
-  </si>
-  <si>
     <t>DE_LA_TORRE</t>
   </si>
   <si>
     <t>MARGARET EVELYN</t>
+  </si>
+  <si>
+    <t>DE SIMPSON MARJORIE JACQUELINE</t>
+  </si>
+  <si>
+    <t>DE GONZALES MARGARITA</t>
+  </si>
+  <si>
+    <t>DE DE LA BARRERA CARLOTA SOFIA</t>
+  </si>
+  <si>
+    <t>DE DEL PINO ROSALBA</t>
+  </si>
+  <si>
+    <t>DE SIMPSON DORA</t>
+  </si>
+  <si>
+    <t>DE DE LOS RIOS RAMONA</t>
+  </si>
+  <si>
+    <t>DE DE LA HOZ KAREN FERNANDA</t>
+  </si>
+  <si>
+    <t>DE DE VIGO CONSUELO</t>
+  </si>
+  <si>
+    <t>DE DEL VALLE PAULA</t>
+  </si>
+  <si>
+    <t>DE DE LAS CASAS CARLA</t>
+  </si>
+  <si>
+    <t>DE RIVEROS SARA</t>
+  </si>
+  <si>
+    <t>DE DEL_NINO_JESUS MARIANA</t>
+  </si>
+  <si>
+    <t>DE DE LA HOZ LUCERO</t>
+  </si>
+  <si>
+    <t>DE SEMMA FEDERICA</t>
+  </si>
+  <si>
+    <t>DE DE LAS CASAS MARIA</t>
+  </si>
+  <si>
+    <t>DE GARCIA PATRICIA</t>
+  </si>
+  <si>
+    <t>DE DEL_NINO_JESUS JOSEFA</t>
+  </si>
+  <si>
+    <t>DE DEL VALLE MARGARITA</t>
+  </si>
+  <si>
+    <t>DE DE LA MORA LEONOR</t>
+  </si>
+  <si>
+    <t>DE DEL PINO JULIA</t>
+  </si>
+  <si>
+    <t>DE DEL VALLE CECILIA</t>
+  </si>
+  <si>
+    <t>DE GOMEZ LISA MARIE</t>
+  </si>
+  <si>
+    <t>DE LA CUEVA</t>
   </si>
 </sst>
 </file>
@@ -694,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8586E9D3-8C93-4FF0-ADD5-B2B2B4BB3EB8}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:H97"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -742,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -768,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
@@ -788,13 +794,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -820,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -846,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
@@ -872,7 +878,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
@@ -898,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
@@ -918,13 +924,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
@@ -944,13 +950,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
@@ -970,13 +976,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -999,10 +1005,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -1022,13 +1028,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
@@ -1048,13 +1054,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
@@ -1074,13 +1080,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
@@ -1100,13 +1106,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
@@ -1126,13 +1132,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
@@ -1152,13 +1158,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
@@ -1178,13 +1184,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
@@ -1204,13 +1210,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
@@ -1230,13 +1236,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
@@ -1256,13 +1262,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>1</v>
@@ -1274,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1285,10 +1291,10 @@
         <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>1</v>
@@ -1297,10 +1303,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1311,10 +1317,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>1</v>
@@ -1340,7 +1346,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1</v>
@@ -1360,13 +1366,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>1</v>
@@ -1386,13 +1392,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>1</v>
@@ -1412,13 +1418,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1</v>
@@ -1438,13 +1444,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>1</v>
@@ -1464,13 +1470,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>1</v>
@@ -1490,13 +1496,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>1</v>
@@ -1505,10 +1511,10 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1519,10 +1525,10 @@
         <v>15</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>1</v>
@@ -1548,7 +1554,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
@@ -1574,7 +1580,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>1</v>
@@ -1594,13 +1600,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -1620,13 +1626,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>1</v>
@@ -1635,10 +1641,10 @@
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1646,13 +1652,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -1672,11 +1678,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>1</v>
@@ -1685,10 +1691,10 @@
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1696,11 +1702,11 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>1</v>
@@ -1709,10 +1715,10 @@
         <v>1</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1720,11 +1726,11 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1</v>
@@ -1733,10 +1739,10 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,11 +1750,11 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>1</v>
@@ -1757,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1772,13 +1778,13 @@
         <v>14</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>1</v>
@@ -1796,7 +1802,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>1</v>
@@ -1805,10 +1811,10 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1816,11 +1822,11 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>1</v>
@@ -1829,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1840,11 +1846,11 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>1</v>
@@ -1853,10 +1859,10 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1864,11 +1870,11 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>1</v>
@@ -1877,10 +1883,10 @@
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1892,13 +1898,13 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>1</v>
@@ -1913,16 +1919,16 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>1</v>
@@ -1936,11 +1942,11 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>1</v>
@@ -1949,10 +1955,10 @@
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1966,7 +1972,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>1</v>
@@ -1992,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>1</v>
@@ -2012,13 +2018,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>1</v>
@@ -2044,7 +2050,7 @@
         <v>13</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>1</v>
@@ -2070,7 +2076,7 @@
         <v>15</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>1</v>
@@ -2096,7 +2102,7 @@
         <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>1</v>
@@ -2122,7 +2128,7 @@
         <v>19</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>1</v>
@@ -2142,13 +2148,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D57" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>1</v>
@@ -2168,13 +2174,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>1</v>
@@ -2194,13 +2200,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>1</v>
@@ -2223,10 +2229,10 @@
         <v>14</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>1</v>
@@ -2246,13 +2252,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>1</v>
@@ -2272,13 +2278,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>1</v>
@@ -2298,13 +2304,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>1</v>
@@ -2324,13 +2330,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>1</v>
@@ -2350,13 +2356,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>1</v>
@@ -2376,13 +2382,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>1</v>
@@ -2402,13 +2408,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>1</v>
@@ -2428,13 +2434,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>1</v>
@@ -2454,13 +2460,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>1</v>
@@ -2480,13 +2486,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>1</v>
@@ -2498,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2509,10 +2515,10 @@
         <v>18</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>1</v>
@@ -2521,10 +2527,10 @@
         <v>1</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2535,10 +2541,10 @@
         <v>17</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>1</v>
@@ -2564,7 +2570,7 @@
         <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>1</v>
@@ -2584,13 +2590,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>1</v>
@@ -2610,13 +2616,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>1</v>
@@ -2636,13 +2642,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>1</v>
@@ -2662,13 +2668,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>1</v>
@@ -2688,13 +2694,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>1</v>
@@ -2714,13 +2720,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>1</v>
@@ -2729,10 +2735,10 @@
         <v>1</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2743,10 +2749,10 @@
         <v>15</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>1</v>
@@ -2772,7 +2778,7 @@
         <v>15</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>1</v>
@@ -2798,7 +2804,7 @@
         <v>17</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>1</v>
@@ -2818,13 +2824,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>1</v>
@@ -2844,13 +2850,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>1</v>
@@ -2859,10 +2865,10 @@
         <v>1</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -2870,13 +2876,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>1</v>
@@ -2896,11 +2902,11 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>1</v>
@@ -2909,10 +2915,10 @@
         <v>1</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2920,11 +2926,11 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>1</v>
@@ -2933,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2944,11 +2950,11 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>1</v>
@@ -2957,10 +2963,10 @@
         <v>1</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -2968,11 +2974,11 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>1</v>
@@ -2981,10 +2987,10 @@
         <v>1</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,13 +3002,13 @@
         <v>14</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>1</v>
@@ -3020,7 +3026,7 @@
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>1</v>
@@ -3029,10 +3035,10 @@
         <v>1</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3040,11 +3046,11 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>1</v>
@@ -3053,10 +3059,10 @@
         <v>1</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3064,11 +3070,11 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>1</v>
@@ -3077,10 +3083,10 @@
         <v>1</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3088,11 +3094,11 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>1</v>
@@ -3101,10 +3107,10 @@
         <v>1</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3116,13 +3122,13 @@
         <v>8</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>1</v>
@@ -3137,16 +3143,16 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>1</v>
@@ -3160,11 +3166,11 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>1</v>
@@ -3173,10 +3179,10 @@
         <v>1</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>